<commit_message>
Obliczenia do wymaganego transferu
</commit_message>
<xml_diff>
--- a/s5/sieci-proj/zestaw_19.xlsx
+++ b/s5/sieci-proj/zestaw_19.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" xr2:uid="{53008BF6-9B19-4C01-A563-A085ADA6BB1D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1" xr2:uid="{53008BF6-9B19-4C01-A563-A085ADA6BB1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,14 +26,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{1C36CB2F-6775-4B0F-B441-2D6494CC0292}" keepAlive="1" name="Query - Zestaw_19" description="Connection to the 'Zestaw_19' query in the workbook." type="5" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Zestaw_19" description="Connection to the 'Zestaw_19' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Zestaw_19;Extended Properties=&quot;&quot;" command="SELECT * FROM [Zestaw_19]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="92">
   <si>
     <t/>
   </si>
@@ -663,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51B6331-5F2C-466B-AB5A-7F731ACA491A}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,6 +1773,1318 @@
       </c>
       <c r="I50" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6AFB3C-A9E4-4ADA-8424-8BFDFF655767}">
+  <dimension ref="A1:I58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2">
+        <v>58</v>
+      </c>
+      <c r="F6" s="2">
+        <v>66</v>
+      </c>
+      <c r="G6" s="2">
+        <f>SUM(B6:F6)</f>
+        <v>219</v>
+      </c>
+      <c r="H6" s="2">
+        <v>219</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" ref="G7:G14" si="0">SUM(B7:F7)</f>
+        <v>171</v>
+      </c>
+      <c r="H7" s="2">
+        <v>171</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2">
+        <v>63</v>
+      </c>
+      <c r="E8" s="2">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2">
+        <v>57</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="H8" s="2">
+        <v>260</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <v>40</v>
+      </c>
+      <c r="D47" s="1">
+        <v>20</v>
+      </c>
+      <c r="E47" s="1">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1">
+        <v>15</v>
+      </c>
+      <c r="G47" s="1">
+        <v>27</v>
+      </c>
+      <c r="H47" s="1">
+        <v>19</v>
+      </c>
+      <c r="I47" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>40</v>
+      </c>
+      <c r="D48" s="1">
+        <v>20</v>
+      </c>
+      <c r="E48" s="1">
+        <v>51</v>
+      </c>
+      <c r="F48" s="1">
+        <v>15</v>
+      </c>
+      <c r="G48" s="1">
+        <v>25</v>
+      </c>
+      <c r="H48" s="1">
+        <v>23</v>
+      </c>
+      <c r="I48" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1">
+        <v>20</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>15</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>22</v>
+      </c>
+      <c r="I49" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="1">
+        <v>56</v>
+      </c>
+      <c r="C50" s="1">
+        <v>40</v>
+      </c>
+      <c r="D50" s="1">
+        <v>20</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>60</v>
+      </c>
+      <c r="H50" s="1">
+        <v>24</v>
+      </c>
+      <c r="I50" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f>SUM(B47*$I$47,B48*$I$48,B49*$I$49,B50*$I$50)</f>
+        <v>952</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:H51" si="1">SUM(C47*$I$47,C48*$I$48,C49*$I$49,C50*$I$50)</f>
+        <v>26680</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>13340</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>18576</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>9750</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>11208</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>14222</v>
+      </c>
+      <c r="I51">
+        <f>SUM(B51:H51)</f>
+        <v>94728</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1">
+        <v>20</v>
+      </c>
+      <c r="E54" s="1">
+        <v>18</v>
+      </c>
+      <c r="F54" s="1">
+        <v>15</v>
+      </c>
+      <c r="G54" s="1">
+        <v>44</v>
+      </c>
+      <c r="H54" s="1">
+        <v>14</v>
+      </c>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <v>40</v>
+      </c>
+      <c r="D55" s="1">
+        <v>20</v>
+      </c>
+      <c r="E55" s="1">
+        <v>17</v>
+      </c>
+      <c r="F55" s="1">
+        <v>15</v>
+      </c>
+      <c r="G55" s="1">
+        <v>46</v>
+      </c>
+      <c r="H55" s="1">
+        <v>15</v>
+      </c>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>40</v>
+      </c>
+      <c r="D56" s="1">
+        <v>20</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>15</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>30</v>
+      </c>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1">
+        <v>40</v>
+      </c>
+      <c r="D57" s="1">
+        <v>20</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>26</v>
+      </c>
+      <c r="H57" s="1">
+        <v>29</v>
+      </c>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <f>SUM(B54*$I$47,B55*$I$48,B56*$I$49,B57*$I$50)</f>
+        <v>170</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:H58" si="2">SUM(C54*$I$47,C55*$I$48,C56*$I$49,C57*$I$50)</f>
+        <v>26680</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>13340</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>6849</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>9750</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>17944</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="2"/>
+        <v>13924</v>
+      </c>
+      <c r="I58">
+        <f>SUM(B58:H58)</f>
+        <v>88657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>